<commit_message>
Add all fields to account settings based on user type
</commit_message>
<xml_diff>
--- a/med/excel_files/Kliniki.xlsx
+++ b/med/excel_files/Kliniki.xlsx
@@ -339,7 +339,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -391,12 +391,6 @@
       <name val="Roboto"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -425,7 +419,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -466,11 +460,8 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -479,7 +470,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="49" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -789,13 +780,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="15" width="9.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="16" width="28.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="16" width="110.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="16" width="64.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="17" width="31.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="18" width="17.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="15" width="13.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="14" width="9.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="15" width="28.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="15" width="110.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="15" width="64.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="16" width="31.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="17" width="17.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="14" width="13.719285714285713" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
@@ -1282,22 +1273,22 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
-      <c r="A22" s="14"/>
+      <c r="A22" s="10"/>
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
       <c r="E22" s="8"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
-      <c r="A23" s="14"/>
+      <c r="A23" s="10"/>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
       <c r="E23" s="8"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>